<commit_message>
changing fastq names because dots in names break at getBaseName fx
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD67BAB-366B-9445-9B7A-66820F18BCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9209F-A164-4491-ABF8-6EF0315BD39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="3760" windowWidth="44880" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VARV_Metadata" sheetId="9" r:id="rId1"/>
@@ -563,7 +563,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -573,7 +573,7 @@
           <rPr>
             <u/>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -582,7 +582,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="398">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4052,19 +4052,10 @@
     <t>test_field_3</t>
   </si>
   <si>
+    <t>VARV_RZ10_3587_2</t>
+  </si>
+  <si>
     <t>local</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/VARV_RZ10_3587_test_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/VARV_RZ10_3587_test_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/VARV_RZ10_3587.2_test_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>/scicomp/instruments-pure/23-4-631_Illumina-MiSeq-M03083/220622_M03083_0094_000000000-KG73J/Alignment_1/20220624_225908/Fastq/VARV_RZ10_3587.2_test_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -4074,7 +4065,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4301,19 +4292,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4836,6 +4814,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4854,12 +4838,6 @@
     </xf>
     <xf numFmtId="3" fontId="32" fillId="42" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5295,200 +5273,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69788A-8BB8-4090-9E16-DE7573DAAD2C}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="40" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>321</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="X1" s="36" t="s">
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="X1" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AB1" s="38" t="s">
         <v>322</v>
       </c>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="36" t="s">
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="AF1" s="36" t="s">
+      <c r="AF1" s="38" t="s">
         <v>323</v>
       </c>
-      <c r="AO1" s="36" t="s">
+      <c r="AO1" s="38" t="s">
         <v>324</v>
       </c>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="38"/>
-      <c r="AY1" s="38"/>
-    </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="AW1" s="40"/>
+      <c r="AX1" s="40"/>
+      <c r="AY1" s="40"/>
+    </row>
+    <row r="2" spans="1:52" ht="18.75" customHeight="1">
+      <c r="A2" s="41" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>382</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>383</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="41" t="s">
         <v>384</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="41" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="42" t="s">
         <v>385</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="42" t="s">
         <v>386</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="42" t="s">
         <v>387</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="42" t="s">
         <v>388</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="42" t="s">
         <v>389</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="43" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="42" t="s">
         <v>390</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="42" t="s">
         <v>391</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="41" t="s">
         <v>376</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="41" t="s">
         <v>377</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="P2" s="41" t="s">
         <v>374</v>
       </c>
-      <c r="Q2" s="39" t="s">
+      <c r="Q2" s="41" t="s">
         <v>375</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="R2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="U2" s="39" t="s">
+      <c r="U2" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="39" t="s">
+      <c r="V2" s="41" t="s">
         <v>327</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="41" t="s">
+      <c r="X2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="39" t="s">
+      <c r="Y2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="39" t="s">
+      <c r="Z2" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="39" t="s">
+      <c r="AA2" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="41" t="s">
+      <c r="AB2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="39" t="s">
+      <c r="AC2" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="42" t="s">
+      <c r="AD2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="41" t="s">
+      <c r="AE2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="41" t="s">
+      <c r="AF2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="39" t="s">
+      <c r="AG2" s="41" t="s">
         <v>366</v>
       </c>
-      <c r="AH2" s="39" t="s">
+      <c r="AH2" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="AI2" s="39" t="s">
+      <c r="AI2" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="39" t="s">
+      <c r="AJ2" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="39" t="s">
+      <c r="AK2" s="41" t="s">
         <v>318</v>
       </c>
-      <c r="AL2" s="39" t="s">
+      <c r="AL2" s="41" t="s">
         <v>392</v>
       </c>
-      <c r="AM2" s="39" t="s">
+      <c r="AM2" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="AN2" s="39" t="s">
+      <c r="AN2" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="AO2" s="41" t="s">
+      <c r="AO2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="AP2" s="39" t="s">
+      <c r="AP2" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="AQ2" s="39" t="s">
+      <c r="AQ2" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="AR2" s="39" t="s">
+      <c r="AR2" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="AS2" s="39" t="s">
+      <c r="AS2" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="AT2" s="39" t="s">
+      <c r="AT2" s="41" t="s">
         <v>319</v>
       </c>
-      <c r="AU2" s="39" t="s">
+      <c r="AU2" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="AW2" s="42" t="s">
+      <c r="AW2" s="44" t="s">
         <v>393</v>
       </c>
-      <c r="AX2" s="42" t="s">
+      <c r="AX2" s="44" t="s">
         <v>394</v>
       </c>
-      <c r="AY2" s="42" t="s">
+      <c r="AY2" s="44" t="s">
         <v>395</v>
       </c>
-      <c r="AZ2" s="42" t="s">
+      <c r="AZ2" s="44" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52">
       <c r="A3" t="s">
         <v>378</v>
       </c>
@@ -5541,21 +5519,15 @@
         <v>61</v>
       </c>
       <c r="AL3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52">
+      <c r="A4" t="s">
         <v>396</v>
       </c>
-      <c r="AM3" t="s">
-        <v>397</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>380</v>
-      </c>
       <c r="B4" t="s">
-        <v>380</v>
+        <v>396</v>
       </c>
       <c r="E4" t="s">
         <v>369</v>
@@ -5603,26 +5575,20 @@
         <v>61</v>
       </c>
       <c r="AL4" t="s">
-        <v>396</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>399</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52">
       <c r="P5" s="28"/>
       <c r="W5" s="35"/>
       <c r="AF5" s="28"/>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52">
       <c r="P6" s="28"/>
       <c r="W6" s="35"/>
       <c r="AF6" s="28"/>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52">
       <c r="P7" s="28"/>
       <c r="W7" s="35"/>
       <c r="AF7" s="28"/>
@@ -5682,20 +5648,20 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -5718,7 +5684,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -5825,7 +5791,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -5926,7 +5892,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
         <v>364</v>
       </c>
@@ -6024,7 +5990,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35">
       <c r="D5" s="28"/>
       <c r="M5" s="28"/>
       <c r="Q5" s="28"/>
@@ -6032,7 +5998,7 @@
       <c r="U5" s="28"/>
       <c r="AC5" s="28"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35">
       <c r="D6" s="28"/>
       <c r="M6" s="28"/>
       <c r="Q6" s="28"/>
@@ -6040,7 +6006,7 @@
       <c r="U6" s="28"/>
       <c r="AC6" s="28"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35">
       <c r="D7" s="28"/>
       <c r="M7" s="28"/>
       <c r="Q7" s="28"/>
@@ -6048,7 +6014,7 @@
       <c r="U7" s="28"/>
       <c r="AC7" s="28"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35">
       <c r="A8" s="30" t="s">
         <v>337</v>
       </c>
@@ -6061,7 +6027,7 @@
       <c r="U8" s="28"/>
       <c r="AC8" s="28"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
         <v>321</v>
       </c>
@@ -6084,7 +6050,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35">
       <c r="A10" s="18" t="s">
         <v>0</v>
       </c>
@@ -6191,7 +6157,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
         <v>328</v>
       </c>
@@ -6239,7 +6205,7 @@
       <c r="U11" s="28"/>
       <c r="AC11" s="28"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
         <v>338</v>
       </c>
@@ -6281,7 +6247,7 @@
       <c r="U12" s="28"/>
       <c r="AC12" s="28"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35">
       <c r="D13" s="28"/>
       <c r="M13" s="28"/>
       <c r="Q13" s="28"/>
@@ -6289,7 +6255,7 @@
       <c r="U13" s="28"/>
       <c r="AC13" s="28"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35">
       <c r="A14" s="30" t="s">
         <v>343</v>
       </c>
@@ -6302,7 +6268,7 @@
       <c r="U14" s="28"/>
       <c r="AC14" s="28"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
         <v>321</v>
       </c>
@@ -6325,7 +6291,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35">
       <c r="A16" s="18" t="s">
         <v>0</v>
       </c>
@@ -6432,7 +6398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
         <v>344</v>
       </c>
@@ -6511,7 +6477,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
         <v>353</v>
       </c>
@@ -6573,7 +6539,7 @@
       </c>
       <c r="AC18" s="28"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
         <v>354</v>
       </c>
@@ -6623,7 +6589,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35">
       <c r="D20" s="28"/>
       <c r="M20" s="28"/>
       <c r="Q20" s="28"/>
@@ -6631,7 +6597,7 @@
       <c r="U20" s="28"/>
       <c r="AC20" s="28"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35">
       <c r="D21" s="28"/>
       <c r="M21" s="28"/>
       <c r="Q21" s="28"/>
@@ -6639,7 +6605,7 @@
       <c r="U21" s="28"/>
       <c r="AC21" s="28"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35">
       <c r="D22" s="28"/>
       <c r="M22" s="28"/>
       <c r="Q22" s="28"/>
@@ -6647,7 +6613,7 @@
       <c r="U22" s="28"/>
       <c r="AC22" s="28"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -6664,7 +6630,7 @@
       <c r="U23" s="28"/>
       <c r="AC23" s="28"/>
     </row>
-    <row r="24" spans="1:35" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" ht="18.75">
       <c r="A24" s="27"/>
       <c r="B24" s="33" t="s">
         <v>363</v>
@@ -6683,7 +6649,7 @@
       <c r="U24" s="28"/>
       <c r="AC24" s="28"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -6700,7 +6666,7 @@
       <c r="U25" s="28"/>
       <c r="AC25" s="28"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -6717,7 +6683,7 @@
       <c r="U26" s="28"/>
       <c r="AC26" s="28"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -6734,7 +6700,7 @@
       <c r="U27" s="28"/>
       <c r="AC27" s="28"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="D28" s="28"/>
       <c r="M28" s="28"/>
       <c r="Q28" s="28"/>
@@ -6742,7 +6708,7 @@
       <c r="U28" s="28"/>
       <c r="AC28" s="28"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="D29" s="28"/>
       <c r="M29" s="28"/>
       <c r="Q29" s="28"/>
@@ -6750,7 +6716,7 @@
       <c r="U29" s="28"/>
       <c r="AC29" s="28"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35">
       <c r="D30" s="28"/>
       <c r="M30" s="28"/>
       <c r="Q30" s="28"/>
@@ -6808,32 +6774,32 @@
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" thickTop="1" thickBottom="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.1640625" style="24"/>
+    <col min="1" max="1" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="24"/>
     <col min="9" max="9" width="13" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" style="24"/>
-    <col min="11" max="12" width="9.1640625" style="12"/>
-    <col min="13" max="14" width="9.1640625" style="23"/>
-    <col min="15" max="15" width="9.1640625" style="12"/>
-    <col min="16" max="16" width="14.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" style="19"/>
-    <col min="18" max="19" width="9.1640625" style="12"/>
-    <col min="20" max="24" width="9.1640625" style="13"/>
-    <col min="25" max="29" width="9.1640625" style="14"/>
-    <col min="32" max="32" width="9.1640625" style="26"/>
-    <col min="33" max="33" width="23.5" customWidth="1"/>
-    <col min="37" max="38" width="9.1640625" style="13"/>
-    <col min="39" max="39" width="9.1640625" style="14"/>
-    <col min="40" max="40" width="19.83203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="24"/>
+    <col min="11" max="12" width="9.140625" style="12"/>
+    <col min="13" max="14" width="9.140625" style="23"/>
+    <col min="15" max="15" width="9.140625" style="12"/>
+    <col min="16" max="16" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="19"/>
+    <col min="18" max="19" width="9.140625" style="12"/>
+    <col min="20" max="24" width="9.140625" style="13"/>
+    <col min="25" max="29" width="9.140625" style="14"/>
+    <col min="32" max="32" width="9.140625" style="26"/>
+    <col min="33" max="33" width="23.42578125" customWidth="1"/>
+    <col min="37" max="38" width="9.140625" style="13"/>
+    <col min="39" max="39" width="9.140625" style="14"/>
+    <col min="40" max="40" width="19.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="18" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="18" customFormat="1" thickTop="1" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -6955,7 +6921,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" thickTop="1" thickBot="1">
       <c r="A2" s="15" t="s">
         <v>39</v>
       </c>
@@ -7131,18 +7097,18 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7237,7 +7203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -7320,7 +7286,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="O4" s="1"/>
     </row>
   </sheetData>
@@ -7337,14 +7303,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7439,7 +7405,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -7549,25 +7515,25 @@
       <selection activeCell="B71" sqref="B71:C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="5"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -7577,14 +7543,14 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="44"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -7594,14 +7560,14 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -7611,14 +7577,14 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="43"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -7628,14 +7594,14 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -7645,14 +7611,14 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -7662,14 +7628,14 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -7679,14 +7645,14 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -7696,14 +7662,14 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -7713,14 +7679,14 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -7730,14 +7696,14 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -7747,14 +7713,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -7764,14 +7730,14 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -7781,14 +7747,14 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="43"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -7798,14 +7764,14 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -7815,14 +7781,14 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -7832,14 +7798,14 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="43"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -7849,14 +7815,14 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -7866,14 +7832,14 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="43"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -7883,14 +7849,14 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="43"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -7900,14 +7866,14 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="36"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -7917,14 +7883,14 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="43"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -7934,14 +7900,14 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="43"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -7951,14 +7917,14 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="43"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -7968,7 +7934,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" s="5" t="s">
         <v>145</v>
       </c>
@@ -7983,7 +7949,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" s="5" t="s">
         <v>146</v>
       </c>
@@ -8000,7 +7966,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" s="5" t="s">
         <v>148</v>
       </c>
@@ -8017,7 +7983,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
         <v>150</v>
       </c>
@@ -8034,7 +8000,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" s="5" t="s">
         <v>152</v>
       </c>
@@ -8051,7 +8017,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="5" t="s">
         <v>154</v>
       </c>
@@ -8068,7 +8034,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="5" t="s">
         <v>156</v>
       </c>
@@ -8083,7 +8049,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" s="5" t="s">
         <v>157</v>
       </c>
@@ -8100,7 +8066,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" s="5" t="s">
         <v>159</v>
       </c>
@@ -8117,7 +8083,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" s="5" t="s">
         <v>161</v>
       </c>
@@ -8134,7 +8100,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" s="5" t="s">
         <v>163</v>
       </c>
@@ -8149,7 +8115,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="5" t="s">
         <v>164</v>
       </c>
@@ -8164,14 +8130,14 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="43"/>
+      <c r="C37" s="36"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -8181,10 +8147,10 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.75" thickBot="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -8194,14 +8160,14 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1">
       <c r="A39" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="44"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -8211,14 +8177,14 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="43"/>
+      <c r="C40" s="36"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -8228,14 +8194,14 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C41" s="43"/>
+      <c r="C41" s="36"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -8245,14 +8211,14 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="43"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -8262,14 +8228,14 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="43"/>
+      <c r="C43" s="36"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -8279,14 +8245,14 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="43"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -8296,14 +8262,14 @@
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="43"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -8313,7 +8279,7 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="5" t="s">
         <v>179</v>
       </c>
@@ -8328,7 +8294,7 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" s="5" t="s">
         <v>180</v>
       </c>
@@ -8343,14 +8309,14 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C48" s="43"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -8360,10 +8326,10 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1">
       <c r="A49" s="5"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -8373,14 +8339,14 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15.75" thickBot="1">
       <c r="A50" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="43"/>
+      <c r="C50" s="36"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -8390,14 +8356,14 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="43" t="s">
+      <c r="B51" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="C51" s="43"/>
+      <c r="C51" s="36"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -8407,14 +8373,14 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="43"/>
+      <c r="C52" s="36"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -8424,14 +8390,14 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="43"/>
+      <c r="C53" s="36"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -8441,14 +8407,14 @@
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="C54" s="43"/>
+      <c r="C54" s="36"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -8458,14 +8424,14 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="C55" s="43"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -8475,14 +8441,14 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="43"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -8492,14 +8458,14 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="43"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -8509,14 +8475,14 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="43"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -8526,14 +8492,14 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="C59" s="43"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -8543,14 +8509,14 @@
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="43"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -8560,14 +8526,14 @@
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="43"/>
+      <c r="C61" s="36"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -8577,14 +8543,14 @@
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="C62" s="43"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -8594,14 +8560,14 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="43"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -8611,14 +8577,14 @@
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="C64" s="43"/>
+      <c r="C64" s="36"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
@@ -8628,14 +8594,14 @@
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="43"/>
+      <c r="C65" s="36"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -8645,14 +8611,14 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="C66" s="43"/>
+      <c r="C66" s="36"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -8662,14 +8628,14 @@
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="C67" s="43"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -8679,14 +8645,14 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="C68" s="43"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -8696,14 +8662,14 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="43"/>
+      <c r="C69" s="36"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -8713,14 +8679,14 @@
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="C70" s="43"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -8730,14 +8696,14 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B71" s="43" t="s">
+      <c r="B71" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="C71" s="43"/>
+      <c r="C71" s="36"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -8747,14 +8713,14 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="C72" s="43"/>
+      <c r="C72" s="36"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -8764,14 +8730,14 @@
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B73" s="43" t="s">
+      <c r="B73" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="C73" s="43"/>
+      <c r="C73" s="36"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -8781,14 +8747,14 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B74" s="43" t="s">
+      <c r="B74" s="36" t="s">
         <v>228</v>
       </c>
-      <c r="C74" s="43"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -8798,14 +8764,14 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B75" s="43" t="s">
+      <c r="B75" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="C75" s="43"/>
+      <c r="C75" s="36"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -8815,14 +8781,14 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B76" s="43" t="s">
+      <c r="B76" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="C76" s="43"/>
+      <c r="C76" s="36"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -8832,14 +8798,14 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="43"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
@@ -8849,7 +8815,7 @@
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78" s="5" t="s">
         <v>235</v>
       </c>
@@ -8864,7 +8830,7 @@
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11">
       <c r="A79" s="5" t="s">
         <v>236</v>
       </c>
@@ -8879,7 +8845,7 @@
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80" s="5" t="s">
         <v>237</v>
       </c>
@@ -8896,7 +8862,7 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11">
       <c r="A81" s="5" t="s">
         <v>239</v>
       </c>
@@ -8913,7 +8879,7 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="A82" s="5" t="s">
         <v>241</v>
       </c>
@@ -8930,7 +8896,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83" s="5" t="s">
         <v>243</v>
       </c>
@@ -8947,7 +8913,7 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15.75" thickBot="1">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="21"/>
@@ -8960,7 +8926,7 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15.75" thickBot="1">
       <c r="A85" s="6" t="s">
         <v>245</v>
       </c>
@@ -8975,7 +8941,7 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11">
       <c r="A86" s="5" t="s">
         <v>246</v>
       </c>
@@ -9010,7 +8976,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11">
       <c r="A87" s="5" t="s">
         <v>249</v>
       </c>
@@ -9045,7 +9011,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="A88" s="5" t="s">
         <v>255</v>
       </c>
@@ -9076,7 +9042,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="26.25">
       <c r="A89" s="5" t="s">
         <v>253</v>
       </c>
@@ -9107,7 +9073,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="26.25">
       <c r="A90" s="5" t="s">
         <v>250</v>
       </c>
@@ -9136,7 +9102,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="26.25">
       <c r="A91" s="5" t="s">
         <v>248</v>
       </c>
@@ -9161,7 +9127,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11">
       <c r="A92" s="5" t="s">
         <v>247</v>
       </c>
@@ -9184,7 +9150,7 @@
       <c r="J92" s="5"/>
       <c r="K92" s="5"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11">
       <c r="A93" s="5" t="s">
         <v>252</v>
       </c>
@@ -9205,7 +9171,7 @@
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11">
       <c r="A94" s="5" t="s">
         <v>254</v>
       </c>
@@ -9224,7 +9190,7 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11">
       <c r="A95" s="5" t="s">
         <v>251</v>
       </c>
@@ -9243,7 +9209,7 @@
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11">
       <c r="A96" s="5"/>
       <c r="B96" s="21"/>
       <c r="C96" s="21" t="s">
@@ -9260,7 +9226,7 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11">
       <c r="A97" s="5"/>
       <c r="B97" s="21"/>
       <c r="C97" s="21" t="s">
@@ -9275,7 +9241,7 @@
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11">
       <c r="A98" s="5"/>
       <c r="B98" s="21"/>
       <c r="C98" s="21" t="s">
@@ -9290,7 +9256,7 @@
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11">
       <c r="A99" s="5"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21" t="s">
@@ -9305,7 +9271,7 @@
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11">
       <c r="A100" s="5"/>
       <c r="B100" s="21"/>
       <c r="C100" s="11" t="s">
@@ -9320,7 +9286,7 @@
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11">
       <c r="A101" s="5"/>
       <c r="B101" s="21"/>
       <c r="C101" s="10" t="s">
@@ -9335,7 +9301,7 @@
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11">
       <c r="A102" s="5"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21" t="s">
@@ -9350,7 +9316,7 @@
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11">
       <c r="A103" s="5"/>
       <c r="B103" s="21"/>
       <c r="C103" s="21" t="s">
@@ -9365,7 +9331,7 @@
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11">
       <c r="A104" s="5"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21" t="s">
@@ -9380,7 +9346,7 @@
       <c r="J104" s="5"/>
       <c r="K104" s="5"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11">
       <c r="A105" s="5"/>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
@@ -9395,7 +9361,7 @@
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11">
       <c r="A106" s="5"/>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
@@ -9410,7 +9376,7 @@
       <c r="J106" s="5"/>
       <c r="K106" s="5"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11">
       <c r="A107" s="5"/>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
@@ -9427,12 +9393,51 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -9445,51 +9450,12 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix variola -add filenames to metadata
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B9209F-A164-4491-ABF8-6EF0315BD39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82661B3-1BCA-4112-81D4-DBBF5A5F992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="402">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4056,6 +4056,18 @@
   </si>
   <si>
     <t>local</t>
+  </si>
+  <si>
+    <t>./VARV_RZ10_3587_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>./VARV_RZ10_3587_2_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>./VARV_RZ10_3587_2_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>./VARV_RZ10_3587_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -5273,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69788A-8BB8-4090-9E16-DE7573DAAD2C}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5521,6 +5533,12 @@
       <c r="AL3" t="s">
         <v>397</v>
       </c>
+      <c r="AM3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" t="s">
@@ -5576,6 +5594,12 @@
       </c>
       <c r="AL4" t="s">
         <v>397</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>400</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:52">

</xml_diff>

<commit_message>
remove fasta_file_name, add fasta_path, correct paths to assets/...
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82661B3-1BCA-4112-81D4-DBBF5A5F992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA86502A-8701-4103-8143-0FD7318A742C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="403">
   <si>
     <t>*sample_name</t>
   </si>
@@ -4068,6 +4068,9 @@
   </si>
   <si>
     <t>./VARV_RZ10_3587_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>oVARV_RZ10_3587</t>
   </si>
 </sst>
 </file>
@@ -4826,12 +4829,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4850,6 +4847,12 @@
     </xf>
     <xf numFmtId="3" fontId="32" fillId="42" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5285,8 +5288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69788A-8BB8-4090-9E16-DE7573DAAD2C}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5298,189 +5301,189 @@
       <c r="A1" t="s">
         <v>321</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="36" t="s">
         <v>317</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="X1" s="38" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="X1" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="AB1" s="38" t="s">
+      <c r="AB1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="38" t="s">
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="AF1" s="38" t="s">
+      <c r="AF1" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="AO1" s="38" t="s">
+      <c r="AO1" s="36" t="s">
         <v>324</v>
       </c>
-      <c r="AW1" s="40"/>
-      <c r="AX1" s="40"/>
-      <c r="AY1" s="40"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="38"/>
     </row>
     <row r="2" spans="1:52" ht="18.75" customHeight="1">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="39" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="39" t="s">
         <v>382</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="39" t="s">
         <v>383</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="39" t="s">
         <v>384</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="39" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="40" t="s">
         <v>385</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="40" t="s">
         <v>386</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="40" t="s">
         <v>387</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="40" t="s">
         <v>388</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="40" t="s">
         <v>389</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="41" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="40" t="s">
         <v>390</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="40" t="s">
         <v>391</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="39" t="s">
         <v>376</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="39" t="s">
         <v>377</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="Q2" s="39" t="s">
         <v>375</v>
       </c>
-      <c r="R2" s="41" t="s">
+      <c r="R2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="41" t="s">
+      <c r="T2" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="U2" s="41" t="s">
+      <c r="U2" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="V2" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="W2" s="41" t="s">
+      <c r="W2" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="43" t="s">
+      <c r="X2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="41" t="s">
+      <c r="Y2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="41" t="s">
+      <c r="Z2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="41" t="s">
+      <c r="AA2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="43" t="s">
+      <c r="AB2" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="41" t="s">
+      <c r="AC2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="AD2" s="44" t="s">
+      <c r="AD2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="43" t="s">
+      <c r="AE2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="43" t="s">
+      <c r="AF2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="41" t="s">
+      <c r="AG2" s="39" t="s">
         <v>366</v>
       </c>
-      <c r="AH2" s="41" t="s">
+      <c r="AH2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="AI2" s="41" t="s">
+      <c r="AI2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="41" t="s">
+      <c r="AJ2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="AK2" s="41" t="s">
+      <c r="AK2" s="39" t="s">
         <v>318</v>
       </c>
-      <c r="AL2" s="41" t="s">
+      <c r="AL2" s="39" t="s">
         <v>392</v>
       </c>
-      <c r="AM2" s="41" t="s">
+      <c r="AM2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="AN2" s="41" t="s">
+      <c r="AN2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="AO2" s="43" t="s">
+      <c r="AO2" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="AP2" s="41" t="s">
+      <c r="AP2" s="39" t="s">
         <v>367</v>
       </c>
-      <c r="AQ2" s="41" t="s">
+      <c r="AQ2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AR2" s="41" t="s">
+      <c r="AR2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="AS2" s="41" t="s">
+      <c r="AS2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="AT2" s="41" t="s">
+      <c r="AT2" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="AU2" s="41" t="s">
+      <c r="AU2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="AW2" s="44" t="s">
+      <c r="AW2" s="42" t="s">
         <v>393</v>
       </c>
-      <c r="AX2" s="44" t="s">
+      <c r="AX2" s="42" t="s">
         <v>394</v>
       </c>
-      <c r="AY2" s="44" t="s">
+      <c r="AY2" s="42" t="s">
         <v>395</v>
       </c>
-      <c r="AZ2" s="44" t="s">
+      <c r="AZ2" s="42" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s">
         <v>378</v>
@@ -7556,8 +7559,8 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="5"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -7571,10 +7574,10 @@
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="37"/>
+      <c r="C2" s="44"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -7588,10 +7591,10 @@
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -7605,10 +7608,10 @@
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -7622,10 +7625,10 @@
       <c r="A5" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -7639,10 +7642,10 @@
       <c r="A6" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -7656,10 +7659,10 @@
       <c r="A7" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -7673,10 +7676,10 @@
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -7690,10 +7693,10 @@
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -7707,10 +7710,10 @@
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -7724,10 +7727,10 @@
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -7741,10 +7744,10 @@
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -7758,10 +7761,10 @@
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -7775,10 +7778,10 @@
       <c r="A14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -7792,10 +7795,10 @@
       <c r="A15" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -7809,10 +7812,10 @@
       <c r="A16" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -7826,10 +7829,10 @@
       <c r="A17" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -7843,10 +7846,10 @@
       <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -7860,10 +7863,10 @@
       <c r="A19" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -7877,10 +7880,10 @@
       <c r="A20" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -7894,10 +7897,10 @@
       <c r="A21" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -7911,10 +7914,10 @@
       <c r="A22" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -7928,10 +7931,10 @@
       <c r="A23" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -7945,10 +7948,10 @@
       <c r="A24" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="36"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -8158,10 +8161,10 @@
       <c r="A37" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="36"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -8173,8 +8176,8 @@
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -8188,10 +8191,10 @@
       <c r="A39" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="37"/>
+      <c r="C39" s="44"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -8205,10 +8208,10 @@
       <c r="A40" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="C40" s="36"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -8222,10 +8225,10 @@
       <c r="A41" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="C41" s="36"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -8239,10 +8242,10 @@
       <c r="A42" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="C42" s="36"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -8256,10 +8259,10 @@
       <c r="A43" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="C43" s="36"/>
+      <c r="C43" s="43"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -8273,10 +8276,10 @@
       <c r="A44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="C44" s="36"/>
+      <c r="C44" s="43"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -8290,10 +8293,10 @@
       <c r="A45" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="36"/>
+      <c r="C45" s="43"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -8337,10 +8340,10 @@
       <c r="A48" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="C48" s="36"/>
+      <c r="C48" s="43"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -8352,8 +8355,8 @@
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1">
       <c r="A49" s="5"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -8367,10 +8370,10 @@
       <c r="A50" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="36"/>
+      <c r="C50" s="43"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -8384,10 +8387,10 @@
       <c r="A51" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="C51" s="36"/>
+      <c r="C51" s="43"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -8401,10 +8404,10 @@
       <c r="A52" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="36"/>
+      <c r="C52" s="43"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -8418,10 +8421,10 @@
       <c r="A53" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="43" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="36"/>
+      <c r="C53" s="43"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -8435,10 +8438,10 @@
       <c r="A54" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="43" t="s">
         <v>188</v>
       </c>
-      <c r="C54" s="36"/>
+      <c r="C54" s="43"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -8452,10 +8455,10 @@
       <c r="A55" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="C55" s="36"/>
+      <c r="C55" s="43"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -8469,10 +8472,10 @@
       <c r="A56" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="36"/>
+      <c r="C56" s="43"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -8486,10 +8489,10 @@
       <c r="A57" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="36"/>
+      <c r="C57" s="43"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
@@ -8503,10 +8506,10 @@
       <c r="A58" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="36"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -8520,10 +8523,10 @@
       <c r="A59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="C59" s="36"/>
+      <c r="C59" s="43"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -8537,10 +8540,10 @@
       <c r="A60" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="36"/>
+      <c r="C60" s="43"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
@@ -8554,10 +8557,10 @@
       <c r="A61" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="36"/>
+      <c r="C61" s="43"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -8571,10 +8574,10 @@
       <c r="A62" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="C62" s="36"/>
+      <c r="C62" s="43"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
@@ -8588,10 +8591,10 @@
       <c r="A63" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="36"/>
+      <c r="C63" s="43"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
@@ -8605,10 +8608,10 @@
       <c r="A64" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="C64" s="36"/>
+      <c r="C64" s="43"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
@@ -8622,10 +8625,10 @@
       <c r="A65" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="36"/>
+      <c r="C65" s="43"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
@@ -8639,10 +8642,10 @@
       <c r="A66" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="C66" s="36"/>
+      <c r="C66" s="43"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
@@ -8656,10 +8659,10 @@
       <c r="A67" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="C67" s="36"/>
+      <c r="C67" s="43"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
@@ -8673,10 +8676,10 @@
       <c r="A68" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="C68" s="36"/>
+      <c r="C68" s="43"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
@@ -8690,10 +8693,10 @@
       <c r="A69" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="C69" s="36"/>
+      <c r="C69" s="43"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -8707,10 +8710,10 @@
       <c r="A70" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="C70" s="36"/>
+      <c r="C70" s="43"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -8724,10 +8727,10 @@
       <c r="A71" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="B71" s="36" t="s">
+      <c r="B71" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="C71" s="36"/>
+      <c r="C71" s="43"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -8741,10 +8744,10 @@
       <c r="A72" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B72" s="36" t="s">
+      <c r="B72" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="C72" s="36"/>
+      <c r="C72" s="43"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -8758,10 +8761,10 @@
       <c r="A73" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="C73" s="36"/>
+      <c r="C73" s="43"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -8775,10 +8778,10 @@
       <c r="A74" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="B74" s="36" t="s">
+      <c r="B74" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="C74" s="36"/>
+      <c r="C74" s="43"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -8792,10 +8795,10 @@
       <c r="A75" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="B75" s="36" t="s">
+      <c r="B75" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="C75" s="36"/>
+      <c r="C75" s="43"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
@@ -8809,10 +8812,10 @@
       <c r="A76" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B76" s="36" t="s">
+      <c r="B76" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="C76" s="36"/>
+      <c r="C76" s="43"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -8826,10 +8829,10 @@
       <c r="A77" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="C77" s="36"/>
+      <c r="C77" s="43"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
@@ -9417,15 +9420,48 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B58:C58"/>
@@ -9438,48 +9474,15 @@
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
upldated variola test data
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
+++ b/assets/sample_metadata/VARV_metadata_Sample_Run_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyoconnell/Desktop/tostadas/assets/sample_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E45AED-469A-4ECD-86A4-9FF96C9502EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C65A5DC-9906-3A4D-8075-533E815A1040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VARV_Metadata" sheetId="9" r:id="rId1"/>
@@ -61,7 +61,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -97,7 +97,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -395,7 +395,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -442,7 +442,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -452,7 +452,7 @@
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -461,7 +461,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2862,7 +2862,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="411">
   <si>
     <t>*sample_name</t>
   </si>
@@ -3971,9 +3971,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Crystal M. Gigante; Philip Lee; Matthew H. Seabolt; Hui Zhao; Kimberly Wilkins; Andrea McCollum; Christina Hutson; Whitni Davidson; Agam Rao; Rafael Mendoza; Yu Li</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ivar 0.1; samtools 1.7; bwa 0.7.17;  SPAdes 3.13.0; CLC 31</t>
   </si>
   <si>
@@ -3998,15 +3995,9 @@
     <t>host</t>
   </si>
   <si>
-    <t>VARV_RZ10_3587</t>
-  </si>
-  <si>
     <t>Variola virus</t>
   </si>
   <si>
-    <t>VARV_RZ10_3587.2</t>
-  </si>
-  <si>
     <t>ncbi-spuid</t>
   </si>
   <si>
@@ -4049,31 +4040,61 @@
     <t>test_field_3</t>
   </si>
   <si>
-    <t>VARV_RZ10_3587_2</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
     <t>fasta_path</t>
   </si>
   <si>
-    <t>assets/sample_fastas/VARV_RZ10_3587.fasta</t>
-  </si>
-  <si>
-    <t>assets/sample_fastas/VARV_RZ10_3587_2.fasta</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/VARV_RZ10_3587_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/VARV_RZ10_3587_2_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/VARV_RZ10_3587_2_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>assets/sample_fastqs/VARV_RZ10_3587_R2.fastq.gz</t>
+    <t>NC_001611</t>
+  </si>
+  <si>
+    <t>PP405578</t>
+  </si>
+  <si>
+    <t>VARV_PP405578</t>
+  </si>
+  <si>
+    <t>VARV_NC_001611</t>
+  </si>
+  <si>
+    <t>Shchelkunov,S.N., Totmenin,A.V., Sandakhchiev,L.S., Blinov,V.M., Resenchuk,S.M., Olenina,L.V., Chirikova,G.B.</t>
+  </si>
+  <si>
+    <t>National Center for Biotechnology Information, NIH</t>
+  </si>
+  <si>
+    <t>1967-01</t>
+  </si>
+  <si>
+    <t>2024-01</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Gigante,C.M., Zhao,H., Smith,J.G., McGrath,D., Takakuwa,J., Hughes,C., Hutson,C., Li,Y.</t>
+  </si>
+  <si>
+    <t>CDC, DHCPP-PRB</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/variola/NC_001611.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastas/variola/PP405578.fasta</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/variola/NC_001611_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/variola/PP405578_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/variola/NC_001611_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t>assets/sample_fastqs/variola/PP405578_R2.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -4083,7 +4104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4310,6 +4331,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -4933,9 +4967,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4973,7 +5007,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5079,7 +5113,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5221,7 +5255,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5294,16 +5328,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED69788A-8BB8-4090-9E16-DE7573DAAD2C}">
   <dimension ref="A1:AZ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AO5" sqref="AO5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="41" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1">
+    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -5333,57 +5367,57 @@
       <c r="AY1" s="38"/>
       <c r="AZ1" s="38"/>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1">
+    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>378</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>380</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>371</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>381</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="G2" s="40" t="s">
         <v>382</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="H2" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="I2" s="40" t="s">
+        <v>384</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>385</v>
+      </c>
+      <c r="K2" s="41" t="s">
         <v>372</v>
       </c>
-      <c r="F2" s="40" t="s">
-        <v>384</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>385</v>
-      </c>
-      <c r="H2" s="40" t="s">
+      <c r="L2" s="40" t="s">
         <v>386</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="M2" s="40" t="s">
         <v>387</v>
       </c>
-      <c r="J2" s="40" t="s">
-        <v>388</v>
-      </c>
-      <c r="K2" s="41" t="s">
+      <c r="N2" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="O2" s="39" t="s">
+        <v>376</v>
+      </c>
+      <c r="P2" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="40" t="s">
-        <v>389</v>
-      </c>
-      <c r="M2" s="40" t="s">
-        <v>390</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>376</v>
-      </c>
-      <c r="O2" s="39" t="s">
-        <v>377</v>
-      </c>
-      <c r="P2" s="39" t="s">
+      <c r="Q2" s="39" t="s">
         <v>374</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>375</v>
       </c>
       <c r="R2" s="39" t="s">
         <v>12</v>
@@ -5425,7 +5459,7 @@
         <v>29</v>
       </c>
       <c r="AE2" s="43" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="AF2" s="41" t="s">
         <v>2</v>
@@ -5449,7 +5483,7 @@
         <v>318</v>
       </c>
       <c r="AM2" s="39" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AN2" s="39" t="s">
         <v>35</v>
@@ -5479,36 +5513,39 @@
         <v>37</v>
       </c>
       <c r="AX2" s="42" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="AY2" s="42" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="AZ2" s="42" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="3" spans="1:52">
-      <c r="A3" t="s">
-        <v>378</v>
-      </c>
       <c r="B3" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
       <c r="E3" t="s">
-        <v>369</v>
+        <v>398</v>
+      </c>
+      <c r="F3" t="s">
+        <v>399</v>
       </c>
       <c r="K3" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="P3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q3" t="s">
-        <v>346</v>
+        <v>400</v>
       </c>
       <c r="R3" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
       <c r="S3" t="s">
         <v>368</v>
@@ -5517,16 +5554,16 @@
         <v>368</v>
       </c>
       <c r="AB3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AD3">
         <v>247</v>
       </c>
       <c r="AE3" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="AF3" s="35" t="s">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="AG3" t="s">
         <v>310</v>
@@ -5544,33 +5581,36 @@
         <v>61</v>
       </c>
       <c r="AM3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AN3" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="AO3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>395</v>
       </c>
       <c r="B4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F4" t="s">
+        <v>404</v>
+      </c>
+      <c r="K4" t="s">
         <v>395</v>
       </c>
-      <c r="E4" t="s">
-        <v>369</v>
-      </c>
-      <c r="K4" t="s">
-        <v>380</v>
-      </c>
       <c r="P4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="Q4" t="s">
-        <v>346</v>
+        <v>401</v>
       </c>
       <c r="R4" t="s">
         <v>368</v>
@@ -5582,16 +5622,16 @@
         <v>368</v>
       </c>
       <c r="AB4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AD4">
         <v>247</v>
       </c>
       <c r="AE4" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="AF4" s="35" t="s">
-        <v>378</v>
+        <v>395</v>
       </c>
       <c r="AG4" t="s">
         <v>310</v>
@@ -5609,26 +5649,26 @@
         <v>61</v>
       </c>
       <c r="AM4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="AN4" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="AO4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="P5" s="28"/>
       <c r="W5" s="35"/>
       <c r="AG5" s="28"/>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="P6" s="28"/>
       <c r="W6" s="35"/>
       <c r="AG6" s="28"/>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="P7" s="28"/>
       <c r="W7" s="35"/>
       <c r="AG7" s="28"/>
@@ -5688,20 +5728,20 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>321</v>
       </c>
@@ -5724,7 +5764,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -5831,7 +5871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>328</v>
       </c>
@@ -5932,7 +5972,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>364</v>
       </c>
@@ -6030,7 +6070,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D5" s="28"/>
       <c r="M5" s="28"/>
       <c r="Q5" s="28"/>
@@ -6038,7 +6078,7 @@
       <c r="U5" s="28"/>
       <c r="AC5" s="28"/>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D6" s="28"/>
       <c r="M6" s="28"/>
       <c r="Q6" s="28"/>
@@ -6046,7 +6086,7 @@
       <c r="U6" s="28"/>
       <c r="AC6" s="28"/>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D7" s="28"/>
       <c r="M7" s="28"/>
       <c r="Q7" s="28"/>
@@ -6054,7 +6094,7 @@
       <c r="U7" s="28"/>
       <c r="AC7" s="28"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>337</v>
       </c>
@@ -6067,7 +6107,7 @@
       <c r="U8" s="28"/>
       <c r="AC8" s="28"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>321</v>
       </c>
@@ -6090,7 +6130,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>0</v>
       </c>
@@ -6197,7 +6237,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>328</v>
       </c>
@@ -6245,7 +6285,7 @@
       <c r="U11" s="28"/>
       <c r="AC11" s="28"/>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>338</v>
       </c>
@@ -6287,7 +6327,7 @@
       <c r="U12" s="28"/>
       <c r="AC12" s="28"/>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D13" s="28"/>
       <c r="M13" s="28"/>
       <c r="Q13" s="28"/>
@@ -6295,7 +6335,7 @@
       <c r="U13" s="28"/>
       <c r="AC13" s="28"/>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>343</v>
       </c>
@@ -6308,7 +6348,7 @@
       <c r="U14" s="28"/>
       <c r="AC14" s="28"/>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>321</v>
       </c>
@@ -6331,7 +6371,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>0</v>
       </c>
@@ -6438,7 +6478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>344</v>
       </c>
@@ -6517,7 +6557,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>353</v>
       </c>
@@ -6579,7 +6619,7 @@
       </c>
       <c r="AC18" s="28"/>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>354</v>
       </c>
@@ -6629,7 +6669,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D20" s="28"/>
       <c r="M20" s="28"/>
       <c r="Q20" s="28"/>
@@ -6637,7 +6677,7 @@
       <c r="U20" s="28"/>
       <c r="AC20" s="28"/>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D21" s="28"/>
       <c r="M21" s="28"/>
       <c r="Q21" s="28"/>
@@ -6645,7 +6685,7 @@
       <c r="U21" s="28"/>
       <c r="AC21" s="28"/>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D22" s="28"/>
       <c r="M22" s="28"/>
       <c r="Q22" s="28"/>
@@ -6653,7 +6693,7 @@
       <c r="U22" s="28"/>
       <c r="AC22" s="28"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="27"/>
       <c r="C23" s="27"/>
@@ -6670,7 +6710,7 @@
       <c r="U23" s="28"/>
       <c r="AC23" s="28"/>
     </row>
-    <row r="24" spans="1:35" ht="18.75">
+    <row r="24" spans="1:35" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="33" t="s">
         <v>363</v>
@@ -6689,7 +6729,7 @@
       <c r="U24" s="28"/>
       <c r="AC24" s="28"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="27"/>
       <c r="C25" s="27"/>
@@ -6706,7 +6746,7 @@
       <c r="U25" s="28"/>
       <c r="AC25" s="28"/>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -6723,7 +6763,7 @@
       <c r="U26" s="28"/>
       <c r="AC26" s="28"/>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -6740,7 +6780,7 @@
       <c r="U27" s="28"/>
       <c r="AC27" s="28"/>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D28" s="28"/>
       <c r="M28" s="28"/>
       <c r="Q28" s="28"/>
@@ -6748,7 +6788,7 @@
       <c r="U28" s="28"/>
       <c r="AC28" s="28"/>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D29" s="28"/>
       <c r="M29" s="28"/>
       <c r="Q29" s="28"/>
@@ -6756,7 +6796,7 @@
       <c r="U29" s="28"/>
       <c r="AC29" s="28"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="D30" s="28"/>
       <c r="M30" s="28"/>
       <c r="Q30" s="28"/>
@@ -6814,32 +6854,32 @@
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" thickTop="1" thickBottom="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" thickTop="1" thickBottom="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="24"/>
+    <col min="1" max="1" width="14.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="15" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.1640625" style="24"/>
     <col min="9" max="9" width="13" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="24"/>
-    <col min="11" max="12" width="9.140625" style="12"/>
-    <col min="13" max="14" width="9.140625" style="23"/>
-    <col min="15" max="15" width="9.140625" style="12"/>
-    <col min="16" max="16" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="19"/>
-    <col min="18" max="19" width="9.140625" style="12"/>
-    <col min="20" max="24" width="9.140625" style="13"/>
-    <col min="25" max="29" width="9.140625" style="14"/>
-    <col min="32" max="32" width="9.140625" style="26"/>
-    <col min="33" max="33" width="23.42578125" customWidth="1"/>
-    <col min="37" max="38" width="9.140625" style="13"/>
-    <col min="39" max="39" width="9.140625" style="14"/>
-    <col min="40" max="40" width="19.85546875" style="15" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="24"/>
+    <col min="11" max="12" width="9.1640625" style="12"/>
+    <col min="13" max="14" width="9.1640625" style="23"/>
+    <col min="15" max="15" width="9.1640625" style="12"/>
+    <col min="16" max="16" width="14.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="19"/>
+    <col min="18" max="19" width="9.1640625" style="12"/>
+    <col min="20" max="24" width="9.1640625" style="13"/>
+    <col min="25" max="29" width="9.1640625" style="14"/>
+    <col min="32" max="32" width="9.1640625" style="26"/>
+    <col min="33" max="33" width="23.5" customWidth="1"/>
+    <col min="37" max="38" width="9.1640625" style="13"/>
+    <col min="39" max="39" width="9.1640625" style="14"/>
+    <col min="40" max="40" width="19.83203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="18" customFormat="1" thickTop="1" thickBot="1">
+    <row r="1" spans="1:40" s="18" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -6961,7 +7001,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:40" thickTop="1" thickBot="1">
+    <row r="2" spans="1:40" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>39</v>
       </c>
@@ -7137,18 +7177,18 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -7243,7 +7283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -7326,7 +7366,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="O4" s="1"/>
     </row>
   </sheetData>
@@ -7343,14 +7383,14 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7445,7 +7485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -7555,22 +7595,22 @@
       <selection activeCell="B71" sqref="B71:C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -7583,7 +7623,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>100</v>
       </c>
@@ -7600,7 +7640,7 @@
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>102</v>
       </c>
@@ -7617,7 +7657,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>58</v>
       </c>
@@ -7634,7 +7674,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>105</v>
       </c>
@@ -7651,7 +7691,7 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>107</v>
       </c>
@@ -7668,7 +7708,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>109</v>
       </c>
@@ -7685,7 +7725,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>111</v>
       </c>
@@ -7702,7 +7742,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -7719,7 +7759,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -7736,7 +7776,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -7753,7 +7793,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -7770,7 +7810,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -7787,7 +7827,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>123</v>
       </c>
@@ -7804,7 +7844,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>125</v>
       </c>
@@ -7821,7 +7861,7 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>127</v>
       </c>
@@ -7838,7 +7878,7 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>129</v>
       </c>
@@ -7855,7 +7895,7 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
@@ -7872,7 +7912,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>133</v>
       </c>
@@ -7889,7 +7929,7 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>135</v>
       </c>
@@ -7906,7 +7946,7 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>137</v>
       </c>
@@ -7923,7 +7963,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>139</v>
       </c>
@@ -7940,7 +7980,7 @@
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>141</v>
       </c>
@@ -7957,7 +7997,7 @@
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>143</v>
       </c>
@@ -7974,7 +8014,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>145</v>
       </c>
@@ -7989,7 +8029,7 @@
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>146</v>
       </c>
@@ -8006,7 +8046,7 @@
       <c r="J26" s="5"/>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>148</v>
       </c>
@@ -8023,7 +8063,7 @@
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>150</v>
       </c>
@@ -8040,7 +8080,7 @@
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>152</v>
       </c>
@@ -8057,7 +8097,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>154</v>
       </c>
@@ -8074,7 +8114,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>156</v>
       </c>
@@ -8089,7 +8129,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>157</v>
       </c>
@@ -8106,7 +8146,7 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>159</v>
       </c>
@@ -8123,7 +8163,7 @@
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>161</v>
       </c>
@@ -8140,7 +8180,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>163</v>
       </c>
@@ -8155,7 +8195,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>164</v>
       </c>
@@ -8170,7 +8210,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>165</v>
       </c>
@@ -8187,7 +8227,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1">
+    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="44"/>
       <c r="C38" s="44"/>
@@ -8200,7 +8240,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1">
+    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>167</v>
       </c>
@@ -8217,7 +8257,7 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>168</v>
       </c>
@@ -8234,7 +8274,7 @@
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>170</v>
       </c>
@@ -8251,7 +8291,7 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>59</v>
       </c>
@@ -8268,7 +8308,7 @@
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>173</v>
       </c>
@@ -8285,7 +8325,7 @@
       <c r="J43" s="5"/>
       <c r="K43" s="5"/>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>175</v>
       </c>
@@ -8302,7 +8342,7 @@
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>177</v>
       </c>
@@ -8319,7 +8359,7 @@
       <c r="J45" s="5"/>
       <c r="K45" s="5"/>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>179</v>
       </c>
@@ -8334,7 +8374,7 @@
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>180</v>
       </c>
@@ -8349,7 +8389,7 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>165</v>
       </c>
@@ -8366,7 +8406,7 @@
       <c r="J48" s="5"/>
       <c r="K48" s="5"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1">
+    <row r="49" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
@@ -8379,7 +8419,7 @@
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1">
+    <row r="50" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>182</v>
       </c>
@@ -8396,7 +8436,7 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
         <v>60</v>
       </c>
@@ -8413,7 +8453,7 @@
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>184</v>
       </c>
@@ -8430,7 +8470,7 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>186</v>
       </c>
@@ -8447,7 +8487,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>98</v>
       </c>
@@ -8464,7 +8504,7 @@
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>189</v>
       </c>
@@ -8481,7 +8521,7 @@
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>191</v>
       </c>
@@ -8498,7 +8538,7 @@
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>193</v>
       </c>
@@ -8515,7 +8555,7 @@
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>195</v>
       </c>
@@ -8532,7 +8572,7 @@
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>197</v>
       </c>
@@ -8549,7 +8589,7 @@
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>199</v>
       </c>
@@ -8566,7 +8606,7 @@
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>201</v>
       </c>
@@ -8583,7 +8623,7 @@
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>203</v>
       </c>
@@ -8600,7 +8640,7 @@
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>205</v>
       </c>
@@ -8617,7 +8657,7 @@
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>207</v>
       </c>
@@ -8634,7 +8674,7 @@
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>209</v>
       </c>
@@ -8651,7 +8691,7 @@
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>211</v>
       </c>
@@ -8668,7 +8708,7 @@
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>213</v>
       </c>
@@ -8685,7 +8725,7 @@
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>215</v>
       </c>
@@ -8702,7 +8742,7 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>217</v>
       </c>
@@ -8719,7 +8759,7 @@
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>219</v>
       </c>
@@ -8736,7 +8776,7 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>221</v>
       </c>
@@ -8753,7 +8793,7 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>223</v>
       </c>
@@ -8770,7 +8810,7 @@
       <c r="J72" s="5"/>
       <c r="K72" s="5"/>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>225</v>
       </c>
@@ -8787,7 +8827,7 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>227</v>
       </c>
@@ -8804,7 +8844,7 @@
       <c r="J74" s="5"/>
       <c r="K74" s="5"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>229</v>
       </c>
@@ -8821,7 +8861,7 @@
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>231</v>
       </c>
@@ -8838,7 +8878,7 @@
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>233</v>
       </c>
@@ -8855,7 +8895,7 @@
       <c r="J77" s="5"/>
       <c r="K77" s="5"/>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>235</v>
       </c>
@@ -8870,7 +8910,7 @@
       <c r="J78" s="5"/>
       <c r="K78" s="5"/>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>236</v>
       </c>
@@ -8885,7 +8925,7 @@
       <c r="J79" s="5"/>
       <c r="K79" s="5"/>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
         <v>237</v>
       </c>
@@ -8902,7 +8942,7 @@
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>239</v>
       </c>
@@ -8919,7 +8959,7 @@
       <c r="J81" s="5"/>
       <c r="K81" s="5"/>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>241</v>
       </c>
@@ -8936,7 +8976,7 @@
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>243</v>
       </c>
@@ -8953,7 +8993,7 @@
       <c r="J83" s="5"/>
       <c r="K83" s="5"/>
     </row>
-    <row r="84" spans="1:11" ht="15.75" thickBot="1">
+    <row r="84" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="21"/>
@@ -8966,7 +9006,7 @@
       <c r="J84" s="5"/>
       <c r="K84" s="5"/>
     </row>
-    <row r="85" spans="1:11" ht="15.75" thickBot="1">
+    <row r="85" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>245</v>
       </c>
@@ -8981,7 +9021,7 @@
       <c r="J85" s="5"/>
       <c r="K85" s="5"/>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>246</v>
       </c>
@@ -9016,7 +9056,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>249</v>
       </c>
@@ -9051,7 +9091,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" ht="16" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>255</v>
       </c>
@@ -9082,7 +9122,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="26.25">
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>253</v>
       </c>
@@ -9113,7 +9153,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="26.25">
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>250</v>
       </c>
@@ -9142,7 +9182,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="26.25">
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>248</v>
       </c>
@@ -9167,7 +9207,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>247</v>
       </c>
@@ -9190,7 +9230,7 @@
       <c r="J92" s="5"/>
       <c r="K92" s="5"/>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>252</v>
       </c>
@@ -9211,7 +9251,7 @@
       <c r="J93" s="5"/>
       <c r="K93" s="5"/>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>254</v>
       </c>
@@ -9230,7 +9270,7 @@
       <c r="J94" s="5"/>
       <c r="K94" s="5"/>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>251</v>
       </c>
@@ -9249,7 +9289,7 @@
       <c r="J95" s="5"/>
       <c r="K95" s="5"/>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="5"/>
       <c r="B96" s="21"/>
       <c r="C96" s="21" t="s">
@@ -9266,7 +9306,7 @@
       <c r="J96" s="5"/>
       <c r="K96" s="5"/>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="5"/>
       <c r="B97" s="21"/>
       <c r="C97" s="21" t="s">
@@ -9281,7 +9321,7 @@
       <c r="J97" s="5"/>
       <c r="K97" s="5"/>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="5"/>
       <c r="B98" s="21"/>
       <c r="C98" s="21" t="s">
@@ -9296,7 +9336,7 @@
       <c r="J98" s="5"/>
       <c r="K98" s="5"/>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="5"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21" t="s">
@@ -9311,7 +9351,7 @@
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="5"/>
       <c r="B100" s="21"/>
       <c r="C100" s="11" t="s">
@@ -9326,7 +9366,7 @@
       <c r="J100" s="5"/>
       <c r="K100" s="5"/>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="5"/>
       <c r="B101" s="21"/>
       <c r="C101" s="10" t="s">
@@ -9341,7 +9381,7 @@
       <c r="J101" s="5"/>
       <c r="K101" s="5"/>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="5"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21" t="s">
@@ -9356,7 +9396,7 @@
       <c r="J102" s="5"/>
       <c r="K102" s="5"/>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="5"/>
       <c r="B103" s="21"/>
       <c r="C103" s="21" t="s">
@@ -9371,7 +9411,7 @@
       <c r="J103" s="5"/>
       <c r="K103" s="5"/>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="5"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21" t="s">
@@ -9386,7 +9426,7 @@
       <c r="J104" s="5"/>
       <c r="K104" s="5"/>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="5"/>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
@@ -9401,7 +9441,7 @@
       <c r="J105" s="5"/>
       <c r="K105" s="5"/>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="5"/>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
@@ -9416,7 +9456,7 @@
       <c r="J106" s="5"/>
       <c r="K106" s="5"/>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="5"/>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">

</xml_diff>